<commit_message>
controllers and views files initial set-up complete
</commit_message>
<xml_diff>
--- a/planning etc/Planning&progress.xlsx
+++ b/planning etc/Planning&progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelconner/codeclan_work/week_05/ruby_project/planning etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F85A511-5EFE-6A49-808D-707463320848}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABAD012-E0AE-7E46-BBAF-DBDA23769E2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22820" yWindow="460" windowWidth="22800" windowHeight="15840" xr2:uid="{E5A05617-005A-9746-8332-E6CF0C3AEAD1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
   <si>
     <t>app.rb</t>
   </si>
@@ -201,10 +201,19 @@
     <t>controllers/</t>
   </si>
   <si>
-    <t>CRUD actions completed</t>
-  </si>
-  <si>
-    <t>basic instances added</t>
+    <t>MVP actions completed</t>
+  </si>
+  <si>
+    <t>MVP schema completed</t>
+  </si>
+  <si>
+    <t>MVP instances added</t>
+  </si>
+  <si>
+    <t>MVP tests not completed</t>
+  </si>
+  <si>
+    <t>started</t>
   </si>
 </sst>
 </file>
@@ -230,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +270,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -406,24 +421,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -455,8 +464,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,7 +800,7 @@
   <dimension ref="B2:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -783,426 +809,425 @@
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="50" customWidth="1"/>
-    <col min="6" max="6" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="43.33203125" customWidth="1"/>
     <col min="7" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="20" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="12"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G4" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="11"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="18"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="17"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="22"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="35" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="12"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G8" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="35" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="12"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G9" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="37"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="36" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="13"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="19"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="6" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="13"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G15" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="17"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="22"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="19"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="6" t="s">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="11"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="11"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="11"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="44"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="44"/>
+      <c r="C25" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="44"/>
+      <c r="C26" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="47"/>
+      <c r="C27" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="11"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="17"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="22"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="24"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="17"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="22"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="16"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="19"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="17"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="22"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="16"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="16"/>
-      <c r="C25" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="16"/>
-      <c r="C26" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="19"/>
-      <c r="C27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="17"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="22"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G29" s="21" t="s">
+      <c r="G29" s="15" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
controllers and views MVP completed
</commit_message>
<xml_diff>
--- a/planning etc/Planning&progress.xlsx
+++ b/planning etc/Planning&progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelconner/codeclan_work/week_05/ruby_project/planning etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABAD012-E0AE-7E46-BBAF-DBDA23769E2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D75461-B67E-D647-BA9C-51FA171FF2F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22820" yWindow="460" windowWidth="22800" windowHeight="15840" xr2:uid="{E5A05617-005A-9746-8332-E6CF0C3AEAD1}"/>
+    <workbookView xWindow="-22820" yWindow="460" windowWidth="22800" windowHeight="19220" xr2:uid="{E5A05617-005A-9746-8332-E6CF0C3AEAD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="76">
   <si>
     <t>app.rb</t>
   </si>
@@ -214,6 +214,45 @@
   </si>
   <si>
     <t>started</t>
+  </si>
+  <si>
+    <t>MVP completed</t>
+  </si>
+  <si>
+    <t>user_controller.rb</t>
+  </si>
+  <si>
+    <t>users view controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not created </t>
+  </si>
+  <si>
+    <t>users/</t>
+  </si>
+  <si>
+    <t>users page yield</t>
+  </si>
+  <si>
+    <t>not created</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>need to add edit/update for the 3 class'  views</t>
+  </si>
+  <si>
+    <t>need to sort rounding issue on monetary amounts</t>
+  </si>
+  <si>
+    <t>draw up proto persona for dril</t>
+  </si>
+  <si>
+    <t>make slideshow of user journey</t>
+  </si>
+  <si>
+    <t>order changes when editing - sql drops most recent change to the bottom</t>
   </si>
 </sst>
 </file>
@@ -239,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +315,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -421,10 +466,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -442,8 +486,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -477,12 +519,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,15 +845,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FAE3ED-8B44-7A4A-A6A3-1CC10F6765BC}">
-  <dimension ref="B2:G29"/>
+  <dimension ref="B2:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
@@ -814,421 +862,483 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="12"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="3" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="11"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="16"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="36" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="12"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="3" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="12"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="3" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="11"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="16"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="27" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33" t="s">
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="27" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="31"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="27" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="13"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="11"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="16"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="50"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="52" t="s">
+      <c r="B17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="10"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="43" t="s">
+      <c r="G19" s="40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="11"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="42" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="43" t="s">
+      <c r="G20" s="40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="42" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="43" t="s">
+      <c r="G21" s="40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="47"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="42" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="50"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="10"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="43" t="s">
+      <c r="G24" s="40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="11"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="42" t="s">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="41"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="G23" s="43" t="s">
+      <c r="G25" s="40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="44"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="46" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="41"/>
+      <c r="C26" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="42" t="s">
+      <c r="E26" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="43" t="s">
+      <c r="G26" s="40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="44"/>
-      <c r="C25" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="46" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="41"/>
+      <c r="C27" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="42" t="s">
+      <c r="E27" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="43" t="s">
+      <c r="G27" s="40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="44"/>
-      <c r="C26" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="46" t="s">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="41"/>
+      <c r="C28" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="42" t="s">
+      <c r="E28" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="G26" s="43" t="s">
+      <c r="G28" s="40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="47"/>
-      <c r="C27" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="49" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="50"/>
+      <c r="C29" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="42" t="s">
+      <c r="E29" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="10"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="45"/>
+      <c r="D31" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="43" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="11"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G29" s="15" t="s">
+      <c r="G31" s="40" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F39" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F40" s="55" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
capitalization added to views
</commit_message>
<xml_diff>
--- a/planning etc/Planning&progress.xlsx
+++ b/planning etc/Planning&progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelconner/codeclan_work/week_05/ruby_project/planning etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40BC58C-8DDE-2C4D-8315-090349426D0E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAC9D77-4603-5E4D-AC2F-657AAAEC68CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23400" yWindow="1380" windowWidth="22960" windowHeight="15840" xr2:uid="{E5A05617-005A-9746-8332-E6CF0C3AEAD1}"/>
+    <workbookView xWindow="5400" yWindow="500" windowWidth="22960" windowHeight="15840" xr2:uid="{E5A05617-005A-9746-8332-E6CF0C3AEAD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="70">
   <si>
     <t>app.rb</t>
   </si>
@@ -226,9 +226,6 @@
     <t>tags views controller</t>
   </si>
   <si>
-    <t>fix order changes when editing - sql drops most recent change to the bottom - could sort by asc in the SQL</t>
-  </si>
-  <si>
     <t>merchants pages yield</t>
   </si>
   <si>
@@ -239,15 +236,6 @@
   </si>
   <si>
     <t>users pages yield</t>
-  </si>
-  <si>
-    <t>need to add in purchase date capture for new purchases</t>
-  </si>
-  <si>
-    <t>need to sort capitalisation on words</t>
-  </si>
-  <si>
-    <t>error checking for zero entries on web forms</t>
   </si>
 </sst>
 </file>
@@ -836,7 +824,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FAE3ED-8B44-7A4A-A6A3-1CC10F6765BC}">
-  <dimension ref="B2:G41"/>
+  <dimension ref="B2:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
@@ -1215,7 +1203,7 @@
         <v>17</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>56</v>
@@ -1233,7 +1221,7 @@
         <v>17</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>56</v>
@@ -1251,7 +1239,7 @@
         <v>17</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>56</v>
@@ -1269,7 +1257,7 @@
         <v>17</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>56</v>
@@ -1308,35 +1296,17 @@
       <c r="D35" t="s">
         <v>60</v>
       </c>
-      <c r="E35" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E36" t="s">
-        <v>71</v>
-      </c>
+      <c r="E36" s="40"/>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E37" s="40" t="s">
-        <v>72</v>
+      <c r="E37" s="39" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E38" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E39" s="40"/>
-    </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E40" s="39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E41" s="39" t="s">
+      <c r="E38" s="39" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final css refactor completed
</commit_message>
<xml_diff>
--- a/planning etc/Planning&progress.xlsx
+++ b/planning etc/Planning&progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelconner/codeclan_work/week_05/ruby_project/planning etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EA911A-C782-7D46-9557-20BC82832414}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26983642-3101-F546-BA93-581BD4A5052C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23400" yWindow="1320" windowWidth="22960" windowHeight="15840" activeTab="1" xr2:uid="{E5A05617-005A-9746-8332-E6CF0C3AEAD1}"/>
+    <workbookView xWindow="-20320" yWindow="460" windowWidth="19400" windowHeight="15840" activeTab="1" xr2:uid="{E5A05617-005A-9746-8332-E6CF0C3AEAD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
   <si>
     <t>app.rb</t>
   </si>
@@ -151,6 +151,9 @@
     <t>Sunday 16 Dec</t>
   </si>
   <si>
+    <t>Monday 17 Dec</t>
+  </si>
+  <si>
     <t>merchants/</t>
   </si>
   <si>
@@ -187,9 +190,6 @@
     <t>MVP instances added</t>
   </si>
   <si>
-    <t>MVP tests not completed</t>
-  </si>
-  <si>
     <t>MVP completed</t>
   </si>
   <si>
@@ -232,16 +232,25 @@
     <t>ACTIONS</t>
   </si>
   <si>
-    <t>make the dashboard the home page</t>
-  </si>
-  <si>
-    <t>change the wording for Tags, Merchants etc</t>
-  </si>
-  <si>
-    <t>edit purchase page selects are not working!!!!!!!!!</t>
-  </si>
-  <si>
     <t>refactor completed</t>
+  </si>
+  <si>
+    <t>MVP tests  completed</t>
+  </si>
+  <si>
+    <t>establsishing good behaviours</t>
+  </si>
+  <si>
+    <t>tested everything but not necessarily documented in specs - need to grow this to something more fomral</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>design</t>
+  </si>
+  <si>
+    <t>didn’t start design until after models db etc completed - in future would begin this earlier - visualistaion really helps</t>
   </si>
 </sst>
 </file>
@@ -288,7 +297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,12 +324,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -507,11 +510,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -535,14 +537,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -552,9 +546,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="47" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -588,14 +579,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,7 +908,7 @@
   <dimension ref="B2:G41"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -928,42 +922,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29" t="s">
+      <c r="B3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="21" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
@@ -971,16 +965,16 @@
         <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -989,39 +983,39 @@
       <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="8"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="11"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29" t="s">
+      <c r="B7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="9"/>
-      <c r="C8" s="4"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1029,15 +1023,15 @@
         <v>24</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="9"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1045,114 +1039,114 @@
         <v>25</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="8"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="11"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21" t="s">
+      <c r="B12" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>39</v>
+      <c r="F12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>39</v>
+      <c r="F13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>39</v>
+      <c r="F14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>39</v>
+      <c r="F15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="8"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="11"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="32"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1161,39 +1155,39 @@
       <c r="F17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="8"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="11"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29" t="s">
+      <c r="B19" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20" t="s">
         <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="9"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="1" t="s">
         <v>2</v>
       </c>
@@ -1201,15 +1195,15 @@
         <v>59</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="9"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="1" t="s">
         <v>3</v>
       </c>
@@ -1217,57 +1211,57 @@
         <v>60</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14" t="s">
         <v>55</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="8"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="11"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="29" t="s">
+      <c r="B24" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="9"/>
-      <c r="C25" s="4"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="1" t="s">
         <v>17</v>
       </c>
@@ -1275,16 +1269,16 @@
         <v>32</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="9"/>
-      <c r="C26" s="4" t="s">
-        <v>41</v>
+      <c r="B26" s="8"/>
+      <c r="C26" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>17</v>
@@ -1293,16 +1287,16 @@
         <v>61</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="9"/>
-      <c r="C27" s="4" t="s">
-        <v>42</v>
+      <c r="B27" s="8"/>
+      <c r="C27" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
@@ -1311,16 +1305,16 @@
         <v>62</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="9"/>
-      <c r="C28" s="4" t="s">
-        <v>43</v>
+      <c r="B28" s="8"/>
+      <c r="C28" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>17</v>
@@ -1329,87 +1323,87 @@
         <v>63</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="13"/>
-      <c r="C29" s="14" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="8"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="11"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="34" t="s">
+      <c r="B31" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="24"/>
+      <c r="D31" s="25" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G31" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="11" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1421,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293C416B-01EB-204B-9953-F8E55C650BFC}">
-  <dimension ref="B3:I21"/>
+  <dimension ref="B3:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1433,145 +1427,166 @@
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="1.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="42" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43" t="s">
+      <c r="D4" s="31"/>
+      <c r="E4" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="42" t="s">
+      <c r="F4" s="32"/>
+      <c r="G4" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="39"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="39"/>
-      <c r="C6" s="45" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="54" t="s">
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="39"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="39"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="27"/>
     </row>
     <row r="8" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="39"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="39"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="27"/>
     </row>
     <row r="9" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="39"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="39"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="27"/>
     </row>
     <row r="10" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="39"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="39"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="27"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="39"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="39"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="27"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="39"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="39"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="27"/>
     </row>
     <row r="13" spans="2:9" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D19" s="45"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E21" s="3"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
labels for payee and category changed
</commit_message>
<xml_diff>
--- a/planning etc/Planning&progress.xlsx
+++ b/planning etc/Planning&progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelconner/codeclan_work/week_05/ruby_project/planning etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26983642-3101-F546-BA93-581BD4A5052C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB8A78B-D38A-674C-934E-E2A35702F726}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20320" yWindow="460" windowWidth="19400" windowHeight="15840" activeTab="1" xr2:uid="{E5A05617-005A-9746-8332-E6CF0C3AEAD1}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
   <si>
     <t>app.rb</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>didn’t start design until after models db etc completed - in future would begin this earlier - visualistaion really helps</t>
+  </si>
+  <si>
+    <t>stop - do - continue</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1421,7 @@
   <dimension ref="B3:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1550,6 +1553,11 @@
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
     </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D19" s="45"/>
     </row>

</xml_diff>